<commit_message>
modify pre-train agents pool sheet
</commit_message>
<xml_diff>
--- a/misc/Pre-trained agents pool for Continual Hanabi.xlsx
+++ b/misc/Pre-trained agents pool for Continual Hanabi.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1926" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1925" uniqueCount="468">
   <si>
     <t>Name of model</t>
   </si>
@@ -1195,9 +1195,6 @@
   </si>
   <si>
     <t>vdn_op_2p_77142</t>
-  </si>
-  <si>
-    <t>Not actually OP</t>
   </si>
   <si>
     <t>vdn_op_2p_77151</t>
@@ -1435,7 +1432,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1507,6 +1504,9 @@
     </font>
     <font/>
     <font>
+      <color rgb="FF000000"/>
+    </font>
+    <font>
       <b/>
       <color rgb="FFFF0000"/>
     </font>
@@ -1531,7 +1531,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1604,6 +1604,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -5558,13 +5561,11 @@
       <c r="O29" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="P29" s="25" t="s">
-        <v>391</v>
-      </c>
+      <c r="P29" s="26"/>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>142</v>
@@ -5609,7 +5610,7 @@
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>142</v>
@@ -5654,7 +5655,7 @@
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>142</v>
@@ -5699,7 +5700,7 @@
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>142</v>
@@ -6422,7 +6423,7 @@
         <v>8141.0</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I14" s="3">
         <v>102.0</v>
@@ -6463,7 +6464,7 @@
         <v>8151.0</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I15" s="3">
         <v>105.0</v>
@@ -6501,7 +6502,7 @@
         <v>292.0</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I16" s="3">
         <v>106.0</v>
@@ -6539,7 +6540,7 @@
         <v>432.0</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I17" s="3">
         <v>107.0</v>
@@ -6583,7 +6584,7 @@
         <v>891.0</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I18" s="3">
         <v>110.0</v>
@@ -7764,7 +7765,7 @@
     </row>
     <row r="55">
       <c r="A55" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>15</v>
@@ -7809,7 +7810,7 @@
     </row>
     <row r="56">
       <c r="A56" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>15</v>
@@ -7854,7 +7855,7 @@
     </row>
     <row r="57">
       <c r="A57" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>15</v>
@@ -7899,7 +7900,7 @@
     </row>
     <row r="58">
       <c r="A58" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>15</v>
@@ -7944,7 +7945,7 @@
     </row>
     <row r="59">
       <c r="A59" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>15</v>
@@ -7989,7 +7990,7 @@
     </row>
     <row r="60">
       <c r="A60" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>15</v>
@@ -8034,7 +8035,7 @@
     </row>
     <row r="61">
       <c r="A61" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>15</v>
@@ -8079,7 +8080,7 @@
     </row>
     <row r="62">
       <c r="A62" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>15</v>
@@ -8124,7 +8125,7 @@
     </row>
     <row r="63">
       <c r="A63" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>15</v>
@@ -8169,7 +8170,7 @@
     </row>
     <row r="64">
       <c r="A64" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>15</v>
@@ -8214,7 +8215,7 @@
     </row>
     <row r="65">
       <c r="A65" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>15</v>
@@ -8259,7 +8260,7 @@
     </row>
     <row r="66">
       <c r="A66" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>15</v>
@@ -8304,7 +8305,7 @@
     </row>
     <row r="67">
       <c r="A67" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>15</v>
@@ -8349,7 +8350,7 @@
     </row>
     <row r="68">
       <c r="A68" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>15</v>
@@ -8394,7 +8395,7 @@
     </row>
     <row r="69">
       <c r="A69" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>15</v>
@@ -8439,7 +8440,7 @@
     </row>
     <row r="70">
       <c r="A70" s="8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>15</v>
@@ -8484,7 +8485,7 @@
     </row>
     <row r="71">
       <c r="A71" s="8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>15</v>
@@ -8529,7 +8530,7 @@
     </row>
     <row r="72">
       <c r="A72" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>15</v>
@@ -8574,7 +8575,7 @@
     </row>
     <row r="73">
       <c r="A73" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>15</v>
@@ -8619,7 +8620,7 @@
     </row>
     <row r="74">
       <c r="A74" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>15</v>
@@ -8664,7 +8665,7 @@
     </row>
     <row r="75">
       <c r="A75" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>15</v>
@@ -8709,7 +8710,7 @@
     </row>
     <row r="76">
       <c r="A76" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>15</v>
@@ -8754,7 +8755,7 @@
     </row>
     <row r="77">
       <c r="A77" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>15</v>
@@ -8799,7 +8800,7 @@
     </row>
     <row r="78">
       <c r="A78" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>15</v>
@@ -8844,7 +8845,7 @@
     </row>
     <row r="79">
       <c r="A79" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>15</v>
@@ -8889,7 +8890,7 @@
     </row>
     <row r="80">
       <c r="A80" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>15</v>
@@ -8934,7 +8935,7 @@
     </row>
     <row r="81">
       <c r="A81" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>15</v>
@@ -8979,7 +8980,7 @@
     </row>
     <row r="82">
       <c r="A82" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>15</v>
@@ -9024,7 +9025,7 @@
     </row>
     <row r="83">
       <c r="A83" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>15</v>
@@ -9069,7 +9070,7 @@
     </row>
     <row r="84">
       <c r="A84" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>15</v>
@@ -9114,7 +9115,7 @@
     </row>
     <row r="85">
       <c r="A85" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>15</v>
@@ -9159,7 +9160,7 @@
     </row>
     <row r="86">
       <c r="A86" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>15</v>
@@ -9204,7 +9205,7 @@
     </row>
     <row r="87">
       <c r="A87" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>15</v>
@@ -9249,7 +9250,7 @@
     </row>
     <row r="88">
       <c r="A88" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>15</v>
@@ -9294,7 +9295,7 @@
     </row>
     <row r="89">
       <c r="A89" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>15</v>
@@ -9339,7 +9340,7 @@
     </row>
     <row r="90">
       <c r="A90" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>15</v>
@@ -9429,7 +9430,7 @@
     </row>
     <row r="93">
       <c r="A93" s="13" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B93" s="14"/>
       <c r="C93" s="13" t="s">
@@ -9474,7 +9475,7 @@
     </row>
     <row r="94">
       <c r="A94" s="13" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B94" s="14"/>
       <c r="C94" s="3" t="s">
@@ -9519,7 +9520,7 @@
     </row>
     <row r="95">
       <c r="A95" s="13" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B95" s="14"/>
       <c r="C95" s="3" t="s">
@@ -9564,7 +9565,7 @@
     </row>
     <row r="96">
       <c r="A96" s="13" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B96" s="14"/>
       <c r="C96" s="3" t="s">
@@ -9609,7 +9610,7 @@
     </row>
     <row r="97">
       <c r="A97" s="14" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B97" s="14"/>
       <c r="C97" s="14" t="s">
@@ -9655,7 +9656,7 @@
     </row>
     <row r="98">
       <c r="A98" s="13" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B98" s="14"/>
       <c r="C98" s="14" t="s">
@@ -9700,7 +9701,7 @@
     </row>
     <row r="99">
       <c r="A99" s="14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B99" s="14"/>
       <c r="C99" s="14" t="s">
@@ -9746,7 +9747,7 @@
     </row>
     <row r="100">
       <c r="A100" s="14" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B100" s="14"/>
       <c r="C100" s="14" t="s">
@@ -9792,7 +9793,7 @@
     </row>
     <row r="101">
       <c r="A101" s="13" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B101" s="14"/>
       <c r="C101" s="13" t="s">
@@ -9837,7 +9838,7 @@
     </row>
     <row r="102">
       <c r="A102" s="13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B102" s="14"/>
       <c r="C102" s="13" t="s">
@@ -9882,7 +9883,7 @@
     </row>
     <row r="103">
       <c r="A103" s="13" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B103" s="14"/>
       <c r="C103" s="14" t="s">
@@ -9927,7 +9928,7 @@
     </row>
     <row r="104">
       <c r="A104" s="14" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B104" s="14"/>
       <c r="C104" s="14" t="s">
@@ -9973,7 +9974,7 @@
     </row>
     <row r="105">
       <c r="A105" s="14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B105" s="14"/>
       <c r="C105" s="14" t="s">
@@ -10019,7 +10020,7 @@
     </row>
     <row r="106">
       <c r="A106" s="14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B106" s="14"/>
       <c r="C106" s="14" t="s">
@@ -10065,7 +10066,7 @@
     </row>
     <row r="107">
       <c r="A107" s="14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B107" s="14"/>
       <c r="C107" s="14" t="s">
@@ -10111,7 +10112,7 @@
     </row>
     <row r="108">
       <c r="A108" s="13" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B108" s="14"/>
       <c r="C108" s="14" t="s">
@@ -10156,7 +10157,7 @@
     </row>
     <row r="109">
       <c r="A109" s="13" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B109" s="14"/>
       <c r="C109" s="3" t="s">
@@ -10201,7 +10202,7 @@
     </row>
     <row r="110">
       <c r="A110" s="13" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B110" s="14"/>
       <c r="C110" s="3" t="s">
@@ -10246,7 +10247,7 @@
     </row>
     <row r="111">
       <c r="A111" s="13" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B111" s="14"/>
       <c r="C111" s="3" t="s">
@@ -10291,7 +10292,7 @@
     </row>
     <row r="112">
       <c r="A112" s="13" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B112" s="14"/>
       <c r="C112" s="3" t="s">
@@ -10336,7 +10337,7 @@
     </row>
     <row r="113">
       <c r="A113" s="13" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B113" s="14"/>
       <c r="C113" s="3" t="s">
@@ -10381,7 +10382,7 @@
     </row>
     <row r="114">
       <c r="A114" s="14" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B114" s="14"/>
       <c r="C114" s="14" t="s">
@@ -10427,7 +10428,7 @@
     </row>
     <row r="115">
       <c r="A115" s="14" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B115" s="14"/>
       <c r="C115" s="14" t="s">
@@ -10473,7 +10474,7 @@
     </row>
     <row r="116">
       <c r="A116" s="13" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B116" s="14"/>
       <c r="C116" s="3" t="s">
@@ -10518,7 +10519,7 @@
     </row>
     <row r="117">
       <c r="A117" s="13" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B117" s="14"/>
       <c r="C117" s="3" t="s">
@@ -10563,7 +10564,7 @@
     </row>
     <row r="118">
       <c r="A118" s="13" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B118" s="14"/>
       <c r="C118" s="3" t="s">
@@ -10608,7 +10609,7 @@
     </row>
     <row r="119">
       <c r="A119" s="13" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B119" s="14"/>
       <c r="C119" s="3" t="s">
@@ -10653,7 +10654,7 @@
     </row>
     <row r="120">
       <c r="A120" s="14" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B120" s="14"/>
       <c r="C120" s="14" t="s">
@@ -10699,7 +10700,7 @@
     </row>
     <row r="121">
       <c r="A121" s="13" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B121" s="14"/>
       <c r="C121" s="3" t="s">
@@ -10744,7 +10745,7 @@
     </row>
     <row r="122">
       <c r="A122" s="14" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B122" s="14"/>
       <c r="C122" s="14" t="s">
@@ -10790,7 +10791,7 @@
     </row>
     <row r="123">
       <c r="A123" s="14" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B123" s="14"/>
       <c r="C123" s="14" t="s">
@@ -10836,7 +10837,7 @@
     </row>
     <row r="124">
       <c r="A124" s="14" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B124" s="14"/>
       <c r="C124" s="14" t="s">

</xml_diff>